<commit_message>
Adições no documento Sprint BacklogV01 e conclusão da parte do issues
</commit_message>
<xml_diff>
--- a/5_Processo_de_monitoramento_e_controle/Relatório_da_sprint/Sprint_Backlog_1_V01.xlsx
+++ b/5_Processo_de_monitoramento_e_controle/Relatório_da_sprint/Sprint_Backlog_1_V01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="20">
   <si>
     <t>Especificação</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>1h:30min</t>
+  </si>
+  <si>
+    <t>4h</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="B2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +477,9 @@
       <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
versões do projecto Nzayilu-mbandu
Versoes do Módulo de criação de termos
</commit_message>
<xml_diff>
--- a/5_Processo_de_monitoramento_e_controle/Relatório_da_sprint/Sprint_Backlog_1_V01.xlsx
+++ b/5_Processo_de_monitoramento_e_controle/Relatório_da_sprint/Sprint_Backlog_1_V01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="21">
   <si>
     <t>Especificação</t>
   </si>
@@ -55,15 +55,9 @@
     <t>Nsunda</t>
   </si>
   <si>
-    <t>Issue</t>
-  </si>
-  <si>
     <t>Artefato</t>
   </si>
   <si>
-    <t>Moduo do sistema</t>
-  </si>
-  <si>
     <t>Criação de termo</t>
   </si>
   <si>
@@ -74,6 +68,15 @@
   </si>
   <si>
     <t>4h</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>Issue (serviço)</t>
+  </si>
+  <si>
+    <t>Modulo do sistema</t>
   </si>
 </sst>
 </file>
@@ -431,7 +434,7 @@
   <dimension ref="B2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,13 +449,13 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -466,7 +469,7 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -475,10 +478,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
@@ -486,7 +489,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -495,16 +498,18 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -513,16 +518,18 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -531,16 +538,18 @@
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -549,16 +558,18 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -567,16 +578,18 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
@@ -585,16 +598,18 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
@@ -603,16 +618,18 @@
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
@@ -621,16 +638,18 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -639,16 +658,18 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -657,16 +678,18 @@
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
@@ -675,16 +698,18 @@
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
@@ -693,16 +718,18 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>8</v>
@@ -711,16 +738,18 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>8</v>
@@ -729,16 +758,18 @@
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G17" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
@@ -747,16 +778,18 @@
         <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
@@ -765,16 +798,18 @@
         <v>0</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
@@ -783,16 +818,18 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>9</v>
@@ -801,16 +838,18 @@
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="G21" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>9</v>
@@ -819,9 +858,11 @@
         <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>